<commit_message>
updated vendor process - AVCDL product mapping template workbook to correct use of color highlighting
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/templates/vendor process - AVCDL product mapping template.xlsx
+++ b/distribution/reference_documents/templates/vendor process - AVCDL product mapping template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F553F4D-EB2E-E644-BA6F-14D948574292}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24516CA3-254C-D64A-8DAE-82FCE71A42A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="4040" windowWidth="44220" windowHeight="27840" xr2:uid="{1C8FF072-BC4B-9747-8DA7-815499AF0FAF}"/>
+    <workbookView xWindow="13260" yWindow="9580" windowWidth="44220" windowHeight="27840" xr2:uid="{1C8FF072-BC4B-9747-8DA7-815499AF0FAF}"/>
   </bookViews>
   <sheets>
     <sheet name="434 req-AVCDL product" sheetId="1" r:id="rId1"/>
@@ -1337,7 +1337,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1523,73 +1523,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1597,6 +1530,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1620,12 +1556,6 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1644,29 +1574,84 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1679,6 +1664,84 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2004,8 +2067,8 @@
   <dimension ref="A1:BI123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7980" topLeftCell="A82" activePane="bottomLeft"/>
-      <selection activeCell="BG4" sqref="BG4:BI4"/>
+      <pane ySplit="7980" topLeftCell="A4"/>
+      <selection sqref="A1:D4"/>
       <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
@@ -2037,115 +2100,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A1" s="98"/>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="87" t="s">
+      <c r="A1" s="91"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="87" t="s">
+      <c r="W1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="100" t="s">
+      <c r="AE1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="101"/>
-      <c r="AH1" s="101"/>
-      <c r="AI1" s="101"/>
-      <c r="AJ1" s="101"/>
-      <c r="AK1" s="101"/>
-      <c r="AL1" s="101"/>
-      <c r="AM1" s="101"/>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="102"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="78"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="103" t="s">
+      <c r="AQ1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="104"/>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="105"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="81"/>
       <c r="AU1" s="1"/>
-      <c r="AV1" s="87" t="s">
+      <c r="AV1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
       <c r="AY1" s="1"/>
-      <c r="AZ1" s="88" t="s">
+      <c r="AZ1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="89"/>
-      <c r="BC1" s="90"/>
+      <c r="BA1" s="66"/>
+      <c r="BB1" s="66"/>
+      <c r="BC1" s="67"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="BF1" s="1"/>
-      <c r="BG1" s="87" t="s">
+      <c r="BG1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="BH1" s="87"/>
-      <c r="BI1" s="87"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="68"/>
     </row>
     <row r="2" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="91">
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="69">
         <v>1</v>
       </c>
-      <c r="F2" s="92"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="3">
         <v>2</v>
       </c>
       <c r="H2" s="3">
         <v>3</v>
       </c>
-      <c r="I2" s="93">
+      <c r="I2" s="138">
         <v>4</v>
       </c>
-      <c r="J2" s="94"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="4">
         <v>5</v>
       </c>
       <c r="L2" s="3">
         <v>6</v>
       </c>
-      <c r="M2" s="95">
+      <c r="M2" s="73">
         <v>7</v>
       </c>
-      <c r="N2" s="96"/>
+      <c r="N2" s="74"/>
       <c r="O2" s="3">
         <v>8</v>
       </c>
@@ -2156,10 +2219,10 @@
         <v>10</v>
       </c>
       <c r="R2" s="5"/>
-      <c r="S2" s="93">
+      <c r="S2" s="71">
         <v>1</v>
       </c>
-      <c r="T2" s="94"/>
+      <c r="T2" s="72"/>
       <c r="U2" s="6">
         <v>2</v>
       </c>
@@ -2173,11 +2236,11 @@
       <c r="Y2" s="4">
         <v>3</v>
       </c>
-      <c r="Z2" s="97">
+      <c r="Z2" s="75">
         <v>4</v>
       </c>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
       <c r="AC2" s="6">
         <v>5</v>
       </c>
@@ -2267,10 +2330,10 @@
       </c>
     </row>
     <row r="3" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="10">
         <v>1</v>
       </c>
@@ -2283,10 +2346,10 @@
       <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>2</v>
       </c>
       <c r="K3" s="4">
@@ -2428,10 +2491,10 @@
       </c>
     </row>
     <row r="4" spans="1:61" s="20" customFormat="1" ht="329" x14ac:dyDescent="0.2">
-      <c r="A4" s="98"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="99"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="16" t="s">
         <v>10</v>
       </c>
@@ -2561,11 +2624,11 @@
         <v>50</v>
       </c>
       <c r="AY4" s="18"/>
-      <c r="AZ4" s="78" t="s">
+      <c r="AZ4" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="80"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="95"/>
       <c r="BC4" s="19" t="s">
         <v>52</v>
       </c>
@@ -2585,10 +2648,10 @@
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="85" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -2656,8 +2719,8 @@
       <c r="BI5" s="25"/>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="85"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="21" t="s">
         <v>61</v>
       </c>
@@ -2723,8 +2786,8 @@
       <c r="BI6" s="25"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A7" s="82"/>
-      <c r="B7" s="85"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="27" t="s">
         <v>63</v>
       </c>
@@ -2792,8 +2855,8 @@
       <c r="BI7" s="25"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A8" s="82"/>
-      <c r="B8" s="85"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="21" t="s">
         <v>65</v>
       </c>
@@ -2859,8 +2922,8 @@
       <c r="BI8" s="25"/>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A9" s="82"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="21" t="s">
         <v>67</v>
       </c>
@@ -2926,8 +2989,8 @@
       <c r="BI9" s="25"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
-      <c r="B10" s="85"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="21" t="s">
         <v>69</v>
       </c>
@@ -2993,8 +3056,8 @@
       <c r="BI10" s="24"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A11" s="82"/>
-      <c r="B11" s="85"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="27" t="s">
         <v>71</v>
       </c>
@@ -3064,8 +3127,8 @@
       <c r="BI11" s="24"/>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A12" s="82"/>
-      <c r="B12" s="85"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="21" t="s">
         <v>73</v>
       </c>
@@ -3131,8 +3194,8 @@
       <c r="BI12" s="24"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="86"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="21" t="s">
         <v>75</v>
       </c>
@@ -3198,8 +3261,8 @@
       <c r="BI13" s="25"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
-      <c r="B14" s="84" t="s">
+      <c r="A14" s="83"/>
+      <c r="B14" s="85" t="s">
         <v>77</v>
       </c>
       <c r="C14" s="27" t="s">
@@ -3271,8 +3334,8 @@
       <c r="BI14" s="24"/>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A15" s="82"/>
-      <c r="B15" s="86"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="21" t="s">
         <v>73</v>
       </c>
@@ -3338,8 +3401,8 @@
       <c r="BI15" s="24"/>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
-      <c r="B16" s="84" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="85" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -3407,8 +3470,8 @@
       <c r="BI16" s="24"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A17" s="82"/>
-      <c r="B17" s="85"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="21" t="s">
         <v>81</v>
       </c>
@@ -3474,7 +3537,7 @@
       <c r="BI17" s="24"/>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="29" t="s">
         <v>83</v>
       </c>
@@ -3547,7 +3610,7 @@
       <c r="BI18" s="24"/>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A19" s="83"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="32" t="s">
         <v>86</v>
       </c>
@@ -3616,10 +3679,10 @@
       <c r="BI19" s="24"/>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="85" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="27" t="s">
@@ -3689,8 +3752,8 @@
       <c r="BI20" s="24"/>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A21" s="82"/>
-      <c r="B21" s="85"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="21" t="s">
         <v>93</v>
       </c>
@@ -3756,8 +3819,8 @@
       <c r="BI21" s="24"/>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A22" s="82"/>
-      <c r="B22" s="85"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="21" t="s">
         <v>95</v>
       </c>
@@ -3823,8 +3886,8 @@
       <c r="BI22" s="24"/>
     </row>
     <row r="23" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A23" s="82"/>
-      <c r="B23" s="85"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="27" t="s">
         <v>95</v>
       </c>
@@ -3892,8 +3955,8 @@
       <c r="BI23" s="24"/>
     </row>
     <row r="24" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
-      <c r="B24" s="85"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="21" t="s">
         <v>98</v>
       </c>
@@ -3959,8 +4022,8 @@
       <c r="BI24" s="24"/>
     </row>
     <row r="25" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A25" s="82"/>
-      <c r="B25" s="85"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="21" t="s">
         <v>100</v>
       </c>
@@ -4026,8 +4089,8 @@
       <c r="BI25" s="24"/>
     </row>
     <row r="26" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A26" s="82"/>
-      <c r="B26" s="85"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="21" t="s">
         <v>102</v>
       </c>
@@ -4093,8 +4156,8 @@
       <c r="BI26" s="24"/>
     </row>
     <row r="27" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A27" s="82"/>
-      <c r="B27" s="85"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="21" t="s">
         <v>104</v>
       </c>
@@ -4160,8 +4223,8 @@
       <c r="BI27" s="24"/>
     </row>
     <row r="28" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="86"/>
       <c r="C28" s="21" t="s">
         <v>106</v>
       </c>
@@ -4227,8 +4290,8 @@
       <c r="BI28" s="24"/>
     </row>
     <row r="29" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="85"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="21" t="s">
         <v>108</v>
       </c>
@@ -4294,8 +4357,8 @@
       <c r="BI29" s="24"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A30" s="82"/>
-      <c r="B30" s="85"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="86"/>
       <c r="C30" s="21" t="s">
         <v>110</v>
       </c>
@@ -4361,8 +4424,8 @@
       <c r="BI30" s="24"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A31" s="82"/>
-      <c r="B31" s="85"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="21" t="s">
         <v>112</v>
       </c>
@@ -4428,8 +4491,8 @@
       <c r="BI31" s="24"/>
     </row>
     <row r="32" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A32" s="82"/>
-      <c r="B32" s="85"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="21" t="s">
         <v>114</v>
       </c>
@@ -4495,8 +4558,8 @@
       <c r="BI32" s="24"/>
     </row>
     <row r="33" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="85"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="21" t="s">
         <v>116</v>
       </c>
@@ -4562,8 +4625,8 @@
       <c r="BI33" s="24"/>
     </row>
     <row r="34" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
-      <c r="B34" s="85"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="21" t="s">
         <v>118</v>
       </c>
@@ -4629,8 +4692,8 @@
       <c r="BI34" s="24"/>
     </row>
     <row r="35" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A35" s="82"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="21" t="s">
         <v>120</v>
       </c>
@@ -4696,8 +4759,8 @@
       <c r="BI35" s="24"/>
     </row>
     <row r="36" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A36" s="82"/>
-      <c r="B36" s="85"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="21" t="s">
         <v>122</v>
       </c>
@@ -4763,8 +4826,8 @@
       <c r="BI36" s="24"/>
     </row>
     <row r="37" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="85"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="21" t="s">
         <v>124</v>
       </c>
@@ -4830,8 +4893,8 @@
       <c r="BI37" s="24"/>
     </row>
     <row r="38" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A38" s="82"/>
-      <c r="B38" s="85"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="21" t="s">
         <v>126</v>
       </c>
@@ -4897,8 +4960,8 @@
       <c r="BI38" s="24"/>
     </row>
     <row r="39" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A39" s="82"/>
-      <c r="B39" s="86"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="21" t="s">
         <v>128</v>
       </c>
@@ -4964,7 +5027,7 @@
       <c r="BI39" s="24"/>
     </row>
     <row r="40" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A40" s="82"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="33" t="s">
         <v>130</v>
       </c>
@@ -5033,8 +5096,8 @@
       <c r="BI40" s="24"/>
     </row>
     <row r="41" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A41" s="82"/>
-      <c r="B41" s="73" t="s">
+      <c r="A41" s="83"/>
+      <c r="B41" s="88" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="30" t="s">
@@ -5104,8 +5167,8 @@
       <c r="BI41" s="24"/>
     </row>
     <row r="42" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A42" s="82"/>
-      <c r="B42" s="75"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="89"/>
       <c r="C42" s="30" t="s">
         <v>136</v>
       </c>
@@ -5173,8 +5236,8 @@
       <c r="BI42" s="24"/>
     </row>
     <row r="43" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A43" s="82"/>
-      <c r="B43" s="75"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="89"/>
       <c r="C43" s="30" t="s">
         <v>138</v>
       </c>
@@ -5242,8 +5305,8 @@
       <c r="BI43" s="24"/>
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A44" s="82"/>
-      <c r="B44" s="75"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="89"/>
       <c r="C44" s="30" t="s">
         <v>140</v>
       </c>
@@ -5311,8 +5374,8 @@
       <c r="BI44" s="24"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A45" s="82"/>
-      <c r="B45" s="75"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="89"/>
       <c r="C45" s="30" t="s">
         <v>142</v>
       </c>
@@ -5380,8 +5443,8 @@
       <c r="BI45" s="24"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
-      <c r="B46" s="75"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="89"/>
       <c r="C46" s="30" t="s">
         <v>144</v>
       </c>
@@ -5449,8 +5512,8 @@
       <c r="BI46" s="24"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
-      <c r="B47" s="75"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="89"/>
       <c r="C47" s="30" t="s">
         <v>146</v>
       </c>
@@ -5518,8 +5581,8 @@
       <c r="BI47" s="24"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A48" s="82"/>
-      <c r="B48" s="74"/>
+      <c r="A48" s="83"/>
+      <c r="B48" s="90"/>
       <c r="C48" s="30" t="s">
         <v>148</v>
       </c>
@@ -5587,8 +5650,8 @@
       <c r="BI48" s="24"/>
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A49" s="82"/>
-      <c r="B49" s="73" t="s">
+      <c r="A49" s="83"/>
+      <c r="B49" s="88" t="s">
         <v>150</v>
       </c>
       <c r="C49" s="30" t="s">
@@ -5660,8 +5723,8 @@
       <c r="BI49" s="24"/>
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A50" s="83"/>
-      <c r="B50" s="74"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="90"/>
       <c r="C50" s="30" t="s">
         <v>153</v>
       </c>
@@ -5794,10 +5857,10 @@
       <c r="BI51" s="26"/>
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A52" s="69" t="s">
+      <c r="A52" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="B52" s="76" t="s">
+      <c r="B52" s="99" t="s">
         <v>156</v>
       </c>
       <c r="C52" s="30" t="s">
@@ -5869,8 +5932,8 @@
       <c r="BI52" s="24"/>
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A53" s="70"/>
-      <c r="B53" s="77"/>
+      <c r="A53" s="98"/>
+      <c r="B53" s="100"/>
       <c r="C53" s="30" t="s">
         <v>159</v>
       </c>
@@ -5940,7 +6003,7 @@
       <c r="BI53" s="24"/>
     </row>
     <row r="54" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A54" s="70"/>
+      <c r="A54" s="98"/>
       <c r="B54" s="39" t="s">
         <v>161</v>
       </c>
@@ -6009,8 +6072,8 @@
       <c r="BI54" s="24"/>
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A55" s="70"/>
-      <c r="B55" s="73" t="s">
+      <c r="A55" s="98"/>
+      <c r="B55" s="88" t="s">
         <v>164</v>
       </c>
       <c r="C55" s="30" t="s">
@@ -6080,8 +6143,8 @@
       </c>
     </row>
     <row r="56" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A56" s="70"/>
-      <c r="B56" s="75"/>
+      <c r="A56" s="98"/>
+      <c r="B56" s="89"/>
       <c r="C56" s="30" t="s">
         <v>167</v>
       </c>
@@ -6149,8 +6212,8 @@
       </c>
     </row>
     <row r="57" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A57" s="71"/>
-      <c r="B57" s="74"/>
+      <c r="A57" s="97"/>
+      <c r="B57" s="90"/>
       <c r="C57" s="30" t="s">
         <v>169</v>
       </c>
@@ -6281,7 +6344,7 @@
       <c r="BI58" s="26"/>
     </row>
     <row r="59" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="96" t="s">
         <v>171</v>
       </c>
       <c r="B59" s="40" t="s">
@@ -6354,7 +6417,7 @@
       <c r="BI59" s="24"/>
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A60" s="70"/>
+      <c r="A60" s="98"/>
       <c r="B60" s="40" t="s">
         <v>175</v>
       </c>
@@ -6425,7 +6488,7 @@
       <c r="BI60" s="24"/>
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A61" s="70"/>
+      <c r="A61" s="98"/>
       <c r="B61" s="40" t="s">
         <v>178</v>
       </c>
@@ -6498,7 +6561,7 @@
       <c r="BI61" s="24"/>
     </row>
     <row r="62" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A62" s="70"/>
+      <c r="A62" s="98"/>
       <c r="B62" s="40" t="s">
         <v>181</v>
       </c>
@@ -6571,8 +6634,8 @@
       <c r="BI62" s="24"/>
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A63" s="70"/>
-      <c r="B63" s="73" t="s">
+      <c r="A63" s="98"/>
+      <c r="B63" s="88" t="s">
         <v>184</v>
       </c>
       <c r="C63" s="30" t="s">
@@ -6646,8 +6709,8 @@
       <c r="BI63" s="24"/>
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A64" s="70"/>
-      <c r="B64" s="74"/>
+      <c r="A64" s="98"/>
+      <c r="B64" s="90"/>
       <c r="C64" s="30" t="s">
         <v>187</v>
       </c>
@@ -6719,7 +6782,7 @@
       <c r="BI64" s="24"/>
     </row>
     <row r="65" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A65" s="70"/>
+      <c r="A65" s="98"/>
       <c r="B65" s="40" t="s">
         <v>189</v>
       </c>
@@ -6800,7 +6863,7 @@
       <c r="BI65" s="24"/>
     </row>
     <row r="66" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A66" s="71"/>
+      <c r="A66" s="97"/>
       <c r="B66" s="41" t="s">
         <v>192</v>
       </c>
@@ -6940,10 +7003,10 @@
       <c r="BI67" s="26"/>
     </row>
     <row r="68" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="101" t="s">
         <v>196</v>
       </c>
       <c r="C68" s="30" t="s">
@@ -7015,8 +7078,8 @@
       <c r="BI68" s="24"/>
     </row>
     <row r="69" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A69" s="70"/>
-      <c r="B69" s="72"/>
+      <c r="A69" s="98"/>
+      <c r="B69" s="101"/>
       <c r="C69" s="30" t="s">
         <v>199</v>
       </c>
@@ -7086,8 +7149,8 @@
       <c r="BI69" s="24"/>
     </row>
     <row r="70" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A70" s="70"/>
-      <c r="B70" s="72" t="s">
+      <c r="A70" s="98"/>
+      <c r="B70" s="101" t="s">
         <v>201</v>
       </c>
       <c r="C70" s="30" t="s">
@@ -7157,8 +7220,8 @@
       <c r="BI70" s="24"/>
     </row>
     <row r="71" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A71" s="70"/>
-      <c r="B71" s="72"/>
+      <c r="A71" s="98"/>
+      <c r="B71" s="101"/>
       <c r="C71" s="30" t="s">
         <v>204</v>
       </c>
@@ -7228,7 +7291,7 @@
       <c r="BI71" s="24"/>
     </row>
     <row r="72" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A72" s="70"/>
+      <c r="A72" s="98"/>
       <c r="B72" s="40" t="s">
         <v>206</v>
       </c>
@@ -7299,7 +7362,7 @@
       <c r="BI72" s="24"/>
     </row>
     <row r="73" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A73" s="70"/>
+      <c r="A73" s="98"/>
       <c r="B73" s="40" t="s">
         <v>209</v>
       </c>
@@ -7370,7 +7433,7 @@
       <c r="BI73" s="24"/>
     </row>
     <row r="74" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A74" s="70"/>
+      <c r="A74" s="98"/>
       <c r="B74" s="40" t="s">
         <v>212</v>
       </c>
@@ -7441,8 +7504,8 @@
       <c r="BI74" s="24"/>
     </row>
     <row r="75" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A75" s="70"/>
-      <c r="B75" s="72" t="s">
+      <c r="A75" s="98"/>
+      <c r="B75" s="101" t="s">
         <v>215</v>
       </c>
       <c r="C75" s="44" t="s">
@@ -7512,8 +7575,8 @@
       <c r="BI75" s="24"/>
     </row>
     <row r="76" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A76" s="70"/>
-      <c r="B76" s="72"/>
+      <c r="A76" s="98"/>
+      <c r="B76" s="101"/>
       <c r="C76" s="44" t="s">
         <v>218</v>
       </c>
@@ -7581,8 +7644,8 @@
       <c r="BI76" s="24"/>
     </row>
     <row r="77" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A77" s="70"/>
-      <c r="B77" s="72"/>
+      <c r="A77" s="98"/>
+      <c r="B77" s="101"/>
       <c r="C77" s="44" t="s">
         <v>220</v>
       </c>
@@ -7650,7 +7713,7 @@
       <c r="BI77" s="24"/>
     </row>
     <row r="78" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A78" s="71"/>
+      <c r="A78" s="97"/>
       <c r="B78" s="45" t="s">
         <v>222</v>
       </c>
@@ -7721,10 +7784,10 @@
       <c r="BI78" s="24"/>
     </row>
     <row r="79" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A79" s="69" t="s">
+      <c r="A79" s="96" t="s">
         <v>225</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B79" s="88" t="s">
         <v>226</v>
       </c>
       <c r="C79" s="30" t="s">
@@ -7794,8 +7857,8 @@
       <c r="BI79" s="24"/>
     </row>
     <row r="80" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A80" s="70"/>
-      <c r="B80" s="74"/>
+      <c r="A80" s="98"/>
+      <c r="B80" s="90"/>
       <c r="C80" s="30" t="s">
         <v>229</v>
       </c>
@@ -7863,7 +7926,7 @@
       <c r="BI80" s="24"/>
     </row>
     <row r="81" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A81" s="70"/>
+      <c r="A81" s="98"/>
       <c r="B81" s="29" t="s">
         <v>231</v>
       </c>
@@ -7934,8 +7997,8 @@
       <c r="BI81" s="24"/>
     </row>
     <row r="82" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A82" s="70"/>
-      <c r="B82" s="72" t="s">
+      <c r="A82" s="98"/>
+      <c r="B82" s="101" t="s">
         <v>234</v>
       </c>
       <c r="C82" s="44" t="s">
@@ -8005,8 +8068,8 @@
       <c r="BI82" s="24"/>
     </row>
     <row r="83" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A83" s="70"/>
-      <c r="B83" s="72"/>
+      <c r="A83" s="98"/>
+      <c r="B83" s="101"/>
       <c r="C83" s="44" t="s">
         <v>237</v>
       </c>
@@ -8074,7 +8137,7 @@
       <c r="BI83" s="24"/>
     </row>
     <row r="84" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A84" s="70"/>
+      <c r="A84" s="98"/>
       <c r="B84" s="45" t="s">
         <v>239</v>
       </c>
@@ -8147,8 +8210,8 @@
       <c r="BI84" s="24"/>
     </row>
     <row r="85" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A85" s="70"/>
-      <c r="B85" s="73" t="s">
+      <c r="A85" s="98"/>
+      <c r="B85" s="88" t="s">
         <v>242</v>
       </c>
       <c r="C85" s="44" t="s">
@@ -8220,8 +8283,8 @@
       <c r="BI85" s="24"/>
     </row>
     <row r="86" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A86" s="70"/>
-      <c r="B86" s="75"/>
+      <c r="A86" s="98"/>
+      <c r="B86" s="89"/>
       <c r="C86" s="44" t="s">
         <v>245</v>
       </c>
@@ -8291,8 +8354,8 @@
       <c r="BI86" s="24"/>
     </row>
     <row r="87" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A87" s="70"/>
-      <c r="B87" s="74"/>
+      <c r="A87" s="98"/>
+      <c r="B87" s="90"/>
       <c r="C87" s="44" t="s">
         <v>247</v>
       </c>
@@ -8362,7 +8425,7 @@
       <c r="BI87" s="24"/>
     </row>
     <row r="88" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A88" s="70"/>
+      <c r="A88" s="98"/>
       <c r="B88" s="45" t="s">
         <v>249</v>
       </c>
@@ -8437,8 +8500,8 @@
       <c r="BI88" s="24"/>
     </row>
     <row r="89" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A89" s="70"/>
-      <c r="B89" s="73" t="s">
+      <c r="A89" s="98"/>
+      <c r="B89" s="88" t="s">
         <v>252</v>
       </c>
       <c r="C89" s="44" t="s">
@@ -8510,8 +8573,8 @@
       <c r="BI89" s="24"/>
     </row>
     <row r="90" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A90" s="70"/>
-      <c r="B90" s="75"/>
+      <c r="A90" s="98"/>
+      <c r="B90" s="89"/>
       <c r="C90" s="44" t="s">
         <v>255</v>
       </c>
@@ -8581,8 +8644,8 @@
       <c r="BI90" s="24"/>
     </row>
     <row r="91" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A91" s="70"/>
-      <c r="B91" s="75"/>
+      <c r="A91" s="98"/>
+      <c r="B91" s="89"/>
       <c r="C91" s="44" t="s">
         <v>245</v>
       </c>
@@ -8652,8 +8715,8 @@
       <c r="BI91" s="24"/>
     </row>
     <row r="92" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A92" s="71"/>
-      <c r="B92" s="74"/>
+      <c r="A92" s="97"/>
+      <c r="B92" s="90"/>
       <c r="C92" s="44" t="s">
         <v>247</v>
       </c>
@@ -8723,10 +8786,10 @@
       <c r="BI92" s="24"/>
     </row>
     <row r="93" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A93" s="69" t="s">
+      <c r="A93" s="96" t="s">
         <v>257</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B93" s="88" t="s">
         <v>258</v>
       </c>
       <c r="C93" s="44" t="s">
@@ -8796,8 +8859,8 @@
       <c r="BI93" s="24"/>
     </row>
     <row r="94" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A94" s="71"/>
-      <c r="B94" s="74"/>
+      <c r="A94" s="97"/>
+      <c r="B94" s="90"/>
       <c r="C94" s="44" t="s">
         <v>261</v>
       </c>
@@ -8928,10 +8991,10 @@
       <c r="BI95" s="26"/>
     </row>
     <row r="96" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A96" s="69" t="s">
+      <c r="A96" s="96" t="s">
         <v>263</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="101" t="s">
         <v>264</v>
       </c>
       <c r="C96" s="44" t="s">
@@ -9003,8 +9066,8 @@
       <c r="BI96" s="24"/>
     </row>
     <row r="97" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A97" s="70"/>
-      <c r="B97" s="72"/>
+      <c r="A97" s="98"/>
+      <c r="B97" s="101"/>
       <c r="C97" s="44" t="s">
         <v>267</v>
       </c>
@@ -9074,7 +9137,7 @@
       <c r="BI97" s="24"/>
     </row>
     <row r="98" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="71"/>
+      <c r="A98" s="97"/>
       <c r="B98" s="41" t="s">
         <v>269</v>
       </c>
@@ -9144,7 +9207,7 @@
       <c r="BI98" s="24"/>
     </row>
     <row r="99" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A99" s="69" t="s">
+      <c r="A99" s="96" t="s">
         <v>272</v>
       </c>
       <c r="B99" s="45" t="s">
@@ -9217,7 +9280,7 @@
       <c r="BI99" s="24"/>
     </row>
     <row r="100" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A100" s="70"/>
+      <c r="A100" s="98"/>
       <c r="B100" s="41" t="s">
         <v>276</v>
       </c>
@@ -9292,7 +9355,7 @@
       <c r="BI100" s="24"/>
     </row>
     <row r="101" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="71"/>
+      <c r="A101" s="97"/>
       <c r="B101" s="41" t="s">
         <v>279</v>
       </c>
@@ -9362,7 +9425,7 @@
       <c r="BI101" s="24"/>
     </row>
     <row r="102" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="69" t="s">
+      <c r="A102" s="96" t="s">
         <v>282</v>
       </c>
       <c r="B102" s="40" t="s">
@@ -9435,7 +9498,7 @@
       <c r="BI102" s="24"/>
     </row>
     <row r="103" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A103" s="71"/>
+      <c r="A103" s="97"/>
       <c r="B103" s="41" t="s">
         <v>286</v>
       </c>
@@ -9569,7 +9632,7 @@
       <c r="BI104" s="26"/>
     </row>
     <row r="105" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A105" s="69" t="s">
+      <c r="A105" s="96" t="s">
         <v>289</v>
       </c>
       <c r="B105" s="40" t="s">
@@ -9642,7 +9705,7 @@
       <c r="BI105" s="24"/>
     </row>
     <row r="106" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A106" s="70"/>
+      <c r="A106" s="98"/>
       <c r="B106" s="40" t="s">
         <v>293</v>
       </c>
@@ -9713,7 +9776,7 @@
       <c r="BI106" s="24"/>
     </row>
     <row r="107" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A107" s="70"/>
+      <c r="A107" s="98"/>
       <c r="B107" s="40" t="s">
         <v>296</v>
       </c>
@@ -9784,8 +9847,8 @@
       <c r="BI107" s="24"/>
     </row>
     <row r="108" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A108" s="70"/>
-      <c r="B108" s="72" t="s">
+      <c r="A108" s="98"/>
+      <c r="B108" s="101" t="s">
         <v>299</v>
       </c>
       <c r="C108" s="44" t="s">
@@ -9855,8 +9918,8 @@
       <c r="BI108" s="24"/>
     </row>
     <row r="109" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A109" s="70"/>
-      <c r="B109" s="72"/>
+      <c r="A109" s="98"/>
+      <c r="B109" s="101"/>
       <c r="C109" s="44" t="s">
         <v>302</v>
       </c>
@@ -9924,8 +9987,8 @@
       <c r="BI109" s="24"/>
     </row>
     <row r="110" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A110" s="70"/>
-      <c r="B110" s="72"/>
+      <c r="A110" s="98"/>
+      <c r="B110" s="101"/>
       <c r="C110" s="44" t="s">
         <v>304</v>
       </c>
@@ -9993,8 +10056,8 @@
       <c r="BI110" s="24"/>
     </row>
     <row r="111" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A111" s="70"/>
-      <c r="B111" s="72" t="s">
+      <c r="A111" s="98"/>
+      <c r="B111" s="101" t="s">
         <v>306</v>
       </c>
       <c r="C111" s="44" t="s">
@@ -10064,8 +10127,8 @@
       <c r="BI111" s="24"/>
     </row>
     <row r="112" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A112" s="70"/>
-      <c r="B112" s="72"/>
+      <c r="A112" s="98"/>
+      <c r="B112" s="101"/>
       <c r="C112" s="44" t="s">
         <v>309</v>
       </c>
@@ -10133,7 +10196,7 @@
       <c r="BI112" s="24"/>
     </row>
     <row r="113" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A113" s="70"/>
+      <c r="A113" s="98"/>
       <c r="B113" s="40" t="s">
         <v>311</v>
       </c>
@@ -10204,8 +10267,8 @@
       <c r="BI113" s="24"/>
     </row>
     <row r="114" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A114" s="70"/>
-      <c r="B114" s="73" t="s">
+      <c r="A114" s="98"/>
+      <c r="B114" s="88" t="s">
         <v>314</v>
       </c>
       <c r="C114" s="44" t="s">
@@ -10275,8 +10338,8 @@
       <c r="BI114" s="24"/>
     </row>
     <row r="115" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A115" s="70"/>
-      <c r="B115" s="74"/>
+      <c r="A115" s="98"/>
+      <c r="B115" s="90"/>
       <c r="C115" s="44" t="s">
         <v>317</v>
       </c>
@@ -10344,7 +10407,7 @@
       <c r="BI115" s="24"/>
     </row>
     <row r="116" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A116" s="71"/>
+      <c r="A116" s="97"/>
       <c r="B116" s="40" t="s">
         <v>319</v>
       </c>
@@ -10415,18 +10478,18 @@
       <c r="BI116" s="24"/>
     </row>
     <row r="118" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B118" s="65" t="s">
+      <c r="B118" s="102" t="s">
         <v>322</v>
       </c>
-      <c r="C118" s="65"/>
-      <c r="D118" s="65"/>
-      <c r="E118" s="65"/>
-      <c r="F118" s="65"/>
-      <c r="G118" s="65"/>
-      <c r="H118" s="65"/>
-      <c r="I118" s="65"/>
-      <c r="J118" s="65"/>
-      <c r="K118" s="65"/>
+      <c r="C118" s="102"/>
+      <c r="D118" s="102"/>
+      <c r="E118" s="102"/>
+      <c r="F118" s="102"/>
+      <c r="G118" s="102"/>
+      <c r="H118" s="102"/>
+      <c r="I118" s="102"/>
+      <c r="J118" s="102"/>
+      <c r="K118" s="102"/>
       <c r="L118" s="48"/>
       <c r="M118" s="48"/>
       <c r="N118" s="48"/>
@@ -10446,46 +10509,46 @@
       <c r="AB118" s="48"/>
     </row>
     <row r="119" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B119" s="66" t="s">
+      <c r="B119" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
+      <c r="C119" s="103"/>
+      <c r="D119" s="103"/>
+      <c r="E119" s="103"/>
+      <c r="F119" s="103"/>
+      <c r="G119" s="103"/>
+      <c r="H119" s="103"/>
+      <c r="I119" s="103"/>
+      <c r="J119" s="103"/>
+      <c r="K119" s="103"/>
     </row>
     <row r="120" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B120" s="67" t="s">
+      <c r="B120" s="104" t="s">
         <v>324</v>
       </c>
-      <c r="C120" s="67"/>
-      <c r="D120" s="67"/>
-      <c r="E120" s="67"/>
-      <c r="F120" s="67"/>
-      <c r="G120" s="67"/>
-      <c r="H120" s="67"/>
-      <c r="I120" s="67"/>
-      <c r="J120" s="67"/>
-      <c r="K120" s="67"/>
+      <c r="C120" s="104"/>
+      <c r="D120" s="104"/>
+      <c r="E120" s="104"/>
+      <c r="F120" s="104"/>
+      <c r="G120" s="104"/>
+      <c r="H120" s="104"/>
+      <c r="I120" s="104"/>
+      <c r="J120" s="104"/>
+      <c r="K120" s="104"/>
     </row>
     <row r="121" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B121" s="68" t="s">
+      <c r="B121" s="105" t="s">
         <v>325</v>
       </c>
-      <c r="C121" s="68"/>
-      <c r="D121" s="68"/>
-      <c r="E121" s="68"/>
-      <c r="F121" s="68"/>
-      <c r="G121" s="68"/>
-      <c r="H121" s="68"/>
-      <c r="I121" s="68"/>
-      <c r="J121" s="68"/>
-      <c r="K121" s="68"/>
+      <c r="C121" s="105"/>
+      <c r="D121" s="105"/>
+      <c r="E121" s="105"/>
+      <c r="F121" s="105"/>
+      <c r="G121" s="105"/>
+      <c r="H121" s="105"/>
+      <c r="I121" s="105"/>
+      <c r="J121" s="105"/>
+      <c r="K121" s="105"/>
     </row>
     <row r="123" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
@@ -10494,29 +10557,18 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="W1:AC1"/>
-    <mergeCell ref="AE1:AO1"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="A20:A50"/>
-    <mergeCell ref="B20:B39"/>
-    <mergeCell ref="B41:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B118:K118"/>
+    <mergeCell ref="B119:K119"/>
+    <mergeCell ref="B120:K120"/>
+    <mergeCell ref="B121:K121"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A105:A116"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B114:B115"/>
     <mergeCell ref="A93:A94"/>
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="A52:A57"/>
@@ -10533,18 +10585,29 @@
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B118:K118"/>
-    <mergeCell ref="B119:K119"/>
-    <mergeCell ref="B120:K120"/>
-    <mergeCell ref="B121:K121"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A105:A116"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A20:A50"/>
+    <mergeCell ref="B20:B39"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="AV1:AX1"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="AE1:AO1"/>
+    <mergeCell ref="AQ1:AT1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10559,9 +10622,9 @@
   <dimension ref="A1:BI121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="7980" topLeftCell="A3" activePane="bottomLeft"/>
+      <pane ySplit="7980" topLeftCell="A4" activePane="bottomLeft"/>
       <selection activeCell="E3" sqref="E1:BI1048576"/>
-      <selection pane="bottomLeft" activeCell="T122" sqref="T122"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10592,115 +10655,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A1" s="98"/>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="87" t="s">
+      <c r="A1" s="91"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="87" t="s">
+      <c r="W1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="100" t="s">
+      <c r="AE1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="101"/>
-      <c r="AH1" s="101"/>
-      <c r="AI1" s="101"/>
-      <c r="AJ1" s="101"/>
-      <c r="AK1" s="101"/>
-      <c r="AL1" s="101"/>
-      <c r="AM1" s="101"/>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="102"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="78"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="103" t="s">
+      <c r="AQ1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="104"/>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="105"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="81"/>
       <c r="AU1" s="1"/>
-      <c r="AV1" s="87" t="s">
+      <c r="AV1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
       <c r="AY1" s="1"/>
-      <c r="AZ1" s="88" t="s">
+      <c r="AZ1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="89"/>
-      <c r="BC1" s="89"/>
+      <c r="BA1" s="66"/>
+      <c r="BB1" s="66"/>
+      <c r="BC1" s="66"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="BF1" s="1"/>
-      <c r="BG1" s="87" t="s">
+      <c r="BG1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="BH1" s="87"/>
-      <c r="BI1" s="87"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="68"/>
     </row>
     <row r="2" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="107">
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="106">
         <v>1</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="106"/>
       <c r="G2" s="49">
         <v>2</v>
       </c>
       <c r="H2" s="49">
         <v>3</v>
       </c>
-      <c r="I2" s="107">
+      <c r="I2" s="106">
         <v>4</v>
       </c>
-      <c r="J2" s="107"/>
+      <c r="J2" s="106"/>
       <c r="K2" s="49">
         <v>5</v>
       </c>
       <c r="L2" s="49">
         <v>6</v>
       </c>
-      <c r="M2" s="107">
+      <c r="M2" s="106">
         <v>7</v>
       </c>
-      <c r="N2" s="107"/>
+      <c r="N2" s="106"/>
       <c r="O2" s="49">
         <v>8</v>
       </c>
@@ -10711,10 +10774,10 @@
         <v>10</v>
       </c>
       <c r="R2" s="5"/>
-      <c r="S2" s="107">
+      <c r="S2" s="106">
         <v>1</v>
       </c>
-      <c r="T2" s="107"/>
+      <c r="T2" s="106"/>
       <c r="U2" s="49">
         <v>2</v>
       </c>
@@ -10728,11 +10791,11 @@
       <c r="Y2" s="49">
         <v>3</v>
       </c>
-      <c r="Z2" s="107">
+      <c r="Z2" s="106">
         <v>4</v>
       </c>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
       <c r="AC2" s="49">
         <v>5</v>
       </c>
@@ -10822,10 +10885,10 @@
       </c>
     </row>
     <row r="3" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="49">
         <v>1</v>
       </c>
@@ -10983,10 +11046,10 @@
       </c>
     </row>
     <row r="4" spans="1:61" s="20" customFormat="1" ht="329" x14ac:dyDescent="0.2">
-      <c r="A4" s="98"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="99"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="16" t="s">
         <v>10</v>
       </c>
@@ -11116,11 +11179,11 @@
         <v>50</v>
       </c>
       <c r="AY4" s="18"/>
-      <c r="AZ4" s="79" t="s">
+      <c r="AZ4" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="80"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="95"/>
       <c r="BC4" s="50" t="s">
         <v>52</v>
       </c>
@@ -11140,13 +11203,13 @@
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="119" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="22" t="s">
@@ -11211,9 +11274,9 @@
       <c r="BI5" s="25"/>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="21" t="s">
+      <c r="A6" s="83"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="119" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="22" t="s">
@@ -11278,9 +11341,9 @@
       <c r="BI6" s="25"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A7" s="82"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="83"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="121" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="22" t="s">
@@ -11345,9 +11408,9 @@
       <c r="BI7" s="25"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A8" s="82"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="21" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="119" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="22" t="s">
@@ -11412,9 +11475,9 @@
       <c r="BI8" s="25"/>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A9" s="82"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="21" t="s">
+      <c r="A9" s="83"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="119" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="22" t="s">
@@ -11479,9 +11542,9 @@
       <c r="BI9" s="25"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="21" t="s">
+      <c r="A10" s="83"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="119" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="22" t="s">
@@ -11546,9 +11609,9 @@
       <c r="BI10" s="24"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A11" s="82"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="27" t="s">
+      <c r="A11" s="83"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="121" t="s">
         <v>71</v>
       </c>
       <c r="D11" s="22" t="s">
@@ -11613,9 +11676,9 @@
       <c r="BI11" s="24"/>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A12" s="82"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="21" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="119" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="22" t="s">
@@ -11680,9 +11743,9 @@
       <c r="BI12" s="24"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="21" t="s">
+      <c r="A13" s="83"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="119" t="s">
         <v>75</v>
       </c>
       <c r="D13" s="22" t="s">
@@ -11747,11 +11810,11 @@
       <c r="BI13" s="25"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
-      <c r="B14" s="84" t="s">
+      <c r="A14" s="83"/>
+      <c r="B14" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="121" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="22" t="s">
@@ -11816,9 +11879,9 @@
       <c r="BI14" s="24"/>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A15" s="82"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="21" t="s">
+      <c r="A15" s="83"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="119" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="22" t="s">
@@ -11883,11 +11946,11 @@
       <c r="BI15" s="24"/>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
-      <c r="B16" s="84" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="119" t="s">
         <v>79</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -11952,9 +12015,9 @@
       <c r="BI16" s="24"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A17" s="82"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="21" t="s">
+      <c r="A17" s="83"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="119" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="22" t="s">
@@ -12019,11 +12082,11 @@
       <c r="BI17" s="24"/>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="83"/>
+      <c r="B18" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="124" t="s">
         <v>84</v>
       </c>
       <c r="D18" s="22" t="s">
@@ -12088,11 +12151,11 @@
       <c r="BI18" s="24"/>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A19" s="83"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="119" t="s">
         <v>87</v>
       </c>
       <c r="D19" s="22" t="s">
@@ -12157,13 +12220,13 @@
       <c r="BI19" s="24"/>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="121" t="s">
         <v>91</v>
       </c>
       <c r="D20" s="22" t="s">
@@ -12228,9 +12291,9 @@
       <c r="BI20" s="24"/>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A21" s="82"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="21" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="119" t="s">
         <v>93</v>
       </c>
       <c r="D21" s="22" t="s">
@@ -12295,9 +12358,9 @@
       <c r="BI21" s="24"/>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A22" s="82"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="21" t="s">
+      <c r="A22" s="83"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="119" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="22" t="s">
@@ -12362,9 +12425,9 @@
       <c r="BI22" s="24"/>
     </row>
     <row r="23" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A23" s="82"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="27" t="s">
+      <c r="A23" s="83"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="121" t="s">
         <v>95</v>
       </c>
       <c r="D23" s="22" t="s">
@@ -12429,9 +12492,9 @@
       <c r="BI23" s="24"/>
     </row>
     <row r="24" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
-      <c r="B24" s="85"/>
-      <c r="C24" s="21" t="s">
+      <c r="A24" s="83"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="119" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="22" t="s">
@@ -12496,9 +12559,9 @@
       <c r="BI24" s="24"/>
     </row>
     <row r="25" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A25" s="82"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="21" t="s">
+      <c r="A25" s="83"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="119" t="s">
         <v>100</v>
       </c>
       <c r="D25" s="22" t="s">
@@ -12563,9 +12626,9 @@
       <c r="BI25" s="24"/>
     </row>
     <row r="26" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A26" s="82"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="21" t="s">
+      <c r="A26" s="83"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="119" t="s">
         <v>102</v>
       </c>
       <c r="D26" s="22" t="s">
@@ -12630,9 +12693,9 @@
       <c r="BI26" s="24"/>
     </row>
     <row r="27" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A27" s="82"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="21" t="s">
+      <c r="A27" s="83"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="119" t="s">
         <v>104</v>
       </c>
       <c r="D27" s="22" t="s">
@@ -12697,9 +12760,9 @@
       <c r="BI27" s="24"/>
     </row>
     <row r="28" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="21" t="s">
+      <c r="A28" s="83"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="119" t="s">
         <v>106</v>
       </c>
       <c r="D28" s="22" t="s">
@@ -12764,9 +12827,9 @@
       <c r="BI28" s="24"/>
     </row>
     <row r="29" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="21" t="s">
+      <c r="A29" s="83"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="119" t="s">
         <v>108</v>
       </c>
       <c r="D29" s="22" t="s">
@@ -12831,9 +12894,9 @@
       <c r="BI29" s="24"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A30" s="82"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="21" t="s">
+      <c r="A30" s="83"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="119" t="s">
         <v>110</v>
       </c>
       <c r="D30" s="22" t="s">
@@ -12898,9 +12961,9 @@
       <c r="BI30" s="24"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A31" s="82"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="21" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="119" t="s">
         <v>112</v>
       </c>
       <c r="D31" s="22" t="s">
@@ -12965,9 +13028,9 @@
       <c r="BI31" s="24"/>
     </row>
     <row r="32" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A32" s="82"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="21" t="s">
+      <c r="A32" s="83"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="119" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="22" t="s">
@@ -13032,9 +13095,9 @@
       <c r="BI32" s="24"/>
     </row>
     <row r="33" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="21" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="119" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="22" t="s">
@@ -13099,9 +13162,9 @@
       <c r="BI33" s="24"/>
     </row>
     <row r="34" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="21" t="s">
+      <c r="A34" s="83"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="119" t="s">
         <v>118</v>
       </c>
       <c r="D34" s="22" t="s">
@@ -13166,9 +13229,9 @@
       <c r="BI34" s="24"/>
     </row>
     <row r="35" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A35" s="82"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="21" t="s">
+      <c r="A35" s="83"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="119" t="s">
         <v>120</v>
       </c>
       <c r="D35" s="22" t="s">
@@ -13233,9 +13296,9 @@
       <c r="BI35" s="24"/>
     </row>
     <row r="36" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A36" s="82"/>
-      <c r="B36" s="85"/>
-      <c r="C36" s="21" t="s">
+      <c r="A36" s="83"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="119" t="s">
         <v>122</v>
       </c>
       <c r="D36" s="22" t="s">
@@ -13300,9 +13363,9 @@
       <c r="BI36" s="24"/>
     </row>
     <row r="37" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="21" t="s">
+      <c r="A37" s="83"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="119" t="s">
         <v>124</v>
       </c>
       <c r="D37" s="22" t="s">
@@ -13367,9 +13430,9 @@
       <c r="BI37" s="24"/>
     </row>
     <row r="38" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A38" s="82"/>
-      <c r="B38" s="85"/>
-      <c r="C38" s="21" t="s">
+      <c r="A38" s="83"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="119" t="s">
         <v>126</v>
       </c>
       <c r="D38" s="22" t="s">
@@ -13434,9 +13497,9 @@
       <c r="BI38" s="24"/>
     </row>
     <row r="39" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A39" s="82"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="21" t="s">
+      <c r="A39" s="83"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="119" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="22" t="s">
@@ -13501,11 +13564,11 @@
       <c r="BI39" s="24"/>
     </row>
     <row r="40" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A40" s="82"/>
-      <c r="B40" s="33" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="126" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="119" t="s">
         <v>131</v>
       </c>
       <c r="D40" s="22" t="s">
@@ -13570,11 +13633,11 @@
       <c r="BI40" s="24"/>
     </row>
     <row r="41" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A41" s="82"/>
-      <c r="B41" s="73" t="s">
+      <c r="A41" s="83"/>
+      <c r="B41" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="124" t="s">
         <v>134</v>
       </c>
       <c r="D41" s="22" t="s">
@@ -13639,9 +13702,9 @@
       <c r="BI41" s="24"/>
     </row>
     <row r="42" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A42" s="82"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="30" t="s">
+      <c r="A42" s="83"/>
+      <c r="B42" s="128"/>
+      <c r="C42" s="124" t="s">
         <v>136</v>
       </c>
       <c r="D42" s="22" t="s">
@@ -13706,9 +13769,9 @@
       <c r="BI42" s="24"/>
     </row>
     <row r="43" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A43" s="82"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="30" t="s">
+      <c r="A43" s="83"/>
+      <c r="B43" s="128"/>
+      <c r="C43" s="124" t="s">
         <v>138</v>
       </c>
       <c r="D43" s="22" t="s">
@@ -13773,9 +13836,9 @@
       <c r="BI43" s="24"/>
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A44" s="82"/>
-      <c r="B44" s="75"/>
-      <c r="C44" s="30" t="s">
+      <c r="A44" s="83"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="124" t="s">
         <v>140</v>
       </c>
       <c r="D44" s="22" t="s">
@@ -13840,9 +13903,9 @@
       <c r="BI44" s="24"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A45" s="82"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="30" t="s">
+      <c r="A45" s="83"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="124" t="s">
         <v>142</v>
       </c>
       <c r="D45" s="22" t="s">
@@ -13907,9 +13970,9 @@
       <c r="BI45" s="24"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
-      <c r="B46" s="75"/>
-      <c r="C46" s="30" t="s">
+      <c r="A46" s="83"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="124" t="s">
         <v>144</v>
       </c>
       <c r="D46" s="22" t="s">
@@ -13974,9 +14037,9 @@
       <c r="BI46" s="24"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="30" t="s">
+      <c r="A47" s="83"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="124" t="s">
         <v>146</v>
       </c>
       <c r="D47" s="22" t="s">
@@ -14041,9 +14104,9 @@
       <c r="BI47" s="24"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A48" s="82"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="30" t="s">
+      <c r="A48" s="83"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="124" t="s">
         <v>148</v>
       </c>
       <c r="D48" s="22" t="s">
@@ -14108,11 +14171,11 @@
       <c r="BI48" s="24"/>
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A49" s="82"/>
-      <c r="B49" s="73" t="s">
+      <c r="A49" s="83"/>
+      <c r="B49" s="127" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="124" t="s">
         <v>151</v>
       </c>
       <c r="D49" s="22" t="s">
@@ -14177,9 +14240,9 @@
       <c r="BI49" s="24"/>
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A50" s="83"/>
-      <c r="B50" s="74"/>
-      <c r="C50" s="30" t="s">
+      <c r="A50" s="84"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="124" t="s">
         <v>153</v>
       </c>
       <c r="D50" s="22" t="s">
@@ -14307,13 +14370,13 @@
       <c r="BI51" s="26"/>
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A52" s="69" t="s">
+      <c r="A52" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="B52" s="76" t="s">
+      <c r="B52" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="124" t="s">
         <v>157</v>
       </c>
       <c r="D52" s="22" t="s">
@@ -14378,9 +14441,9 @@
       <c r="BI52" s="24"/>
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A53" s="70"/>
-      <c r="B53" s="77"/>
-      <c r="C53" s="30" t="s">
+      <c r="A53" s="98"/>
+      <c r="B53" s="131"/>
+      <c r="C53" s="124" t="s">
         <v>159</v>
       </c>
       <c r="D53" s="22" t="s">
@@ -14445,11 +14508,11 @@
       <c r="BI53" s="24"/>
     </row>
     <row r="54" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A54" s="70"/>
-      <c r="B54" s="39" t="s">
+      <c r="A54" s="98"/>
+      <c r="B54" s="132" t="s">
         <v>161</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="119" t="s">
         <v>162</v>
       </c>
       <c r="D54" s="22" t="s">
@@ -14514,11 +14577,11 @@
       <c r="BI54" s="24"/>
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A55" s="70"/>
-      <c r="B55" s="73" t="s">
+      <c r="A55" s="98"/>
+      <c r="B55" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="124" t="s">
         <v>165</v>
       </c>
       <c r="D55" s="22" t="s">
@@ -14583,9 +14646,9 @@
       <c r="BI55" s="24"/>
     </row>
     <row r="56" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A56" s="70"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="30" t="s">
+      <c r="A56" s="98"/>
+      <c r="B56" s="128"/>
+      <c r="C56" s="124" t="s">
         <v>167</v>
       </c>
       <c r="D56" s="22" t="s">
@@ -14650,9 +14713,9 @@
       <c r="BI56" s="24"/>
     </row>
     <row r="57" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A57" s="71"/>
-      <c r="B57" s="74"/>
-      <c r="C57" s="30" t="s">
+      <c r="A57" s="97"/>
+      <c r="B57" s="129"/>
+      <c r="C57" s="124" t="s">
         <v>169</v>
       </c>
       <c r="D57" s="22" t="s">
@@ -14780,13 +14843,13 @@
       <c r="BI58" s="26"/>
     </row>
     <row r="59" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="96" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="124" t="s">
         <v>173</v>
       </c>
       <c r="D59" s="22" t="s">
@@ -14851,11 +14914,11 @@
       <c r="BI59" s="24"/>
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A60" s="70"/>
-      <c r="B60" s="40" t="s">
+      <c r="A60" s="98"/>
+      <c r="B60" s="133" t="s">
         <v>175</v>
       </c>
-      <c r="C60" s="30" t="s">
+      <c r="C60" s="124" t="s">
         <v>176</v>
       </c>
       <c r="D60" s="22" t="s">
@@ -14920,11 +14983,11 @@
       <c r="BI60" s="24"/>
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A61" s="70"/>
-      <c r="B61" s="40" t="s">
+      <c r="A61" s="98"/>
+      <c r="B61" s="133" t="s">
         <v>178</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="124" t="s">
         <v>179</v>
       </c>
       <c r="D61" s="22" t="s">
@@ -14989,11 +15052,11 @@
       <c r="BI61" s="24"/>
     </row>
     <row r="62" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A62" s="70"/>
-      <c r="B62" s="40" t="s">
+      <c r="A62" s="98"/>
+      <c r="B62" s="133" t="s">
         <v>181</v>
       </c>
-      <c r="C62" s="30" t="s">
+      <c r="C62" s="124" t="s">
         <v>182</v>
       </c>
       <c r="D62" s="22" t="s">
@@ -15058,11 +15121,11 @@
       <c r="BI62" s="24"/>
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A63" s="70"/>
-      <c r="B63" s="73" t="s">
+      <c r="A63" s="98"/>
+      <c r="B63" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="C63" s="124" t="s">
         <v>185</v>
       </c>
       <c r="D63" s="22" t="s">
@@ -15127,9 +15190,9 @@
       <c r="BI63" s="24"/>
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A64" s="70"/>
-      <c r="B64" s="74"/>
-      <c r="C64" s="30" t="s">
+      <c r="A64" s="98"/>
+      <c r="B64" s="129"/>
+      <c r="C64" s="124" t="s">
         <v>187</v>
       </c>
       <c r="D64" s="22" t="s">
@@ -15194,11 +15257,11 @@
       <c r="BI64" s="24"/>
     </row>
     <row r="65" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A65" s="70"/>
-      <c r="B65" s="40" t="s">
+      <c r="A65" s="98"/>
+      <c r="B65" s="133" t="s">
         <v>189</v>
       </c>
-      <c r="C65" s="30" t="s">
+      <c r="C65" s="124" t="s">
         <v>190</v>
       </c>
       <c r="D65" s="22" t="s">
@@ -15263,11 +15326,11 @@
       <c r="BI65" s="24"/>
     </row>
     <row r="66" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A66" s="71"/>
-      <c r="B66" s="41" t="s">
+      <c r="A66" s="97"/>
+      <c r="B66" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="124" t="s">
         <v>193</v>
       </c>
       <c r="D66" s="22" t="s">
@@ -15395,13 +15458,13 @@
       <c r="BI67" s="26"/>
     </row>
     <row r="68" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="C68" s="124" t="s">
         <v>197</v>
       </c>
       <c r="D68" s="22" t="s">
@@ -15466,9 +15529,9 @@
       <c r="BI68" s="24"/>
     </row>
     <row r="69" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A69" s="70"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="30" t="s">
+      <c r="A69" s="98"/>
+      <c r="B69" s="135"/>
+      <c r="C69" s="124" t="s">
         <v>199</v>
       </c>
       <c r="D69" s="22" t="s">
@@ -15533,11 +15596,11 @@
       <c r="BI69" s="24"/>
     </row>
     <row r="70" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A70" s="70"/>
-      <c r="B70" s="72" t="s">
+      <c r="A70" s="98"/>
+      <c r="B70" s="135" t="s">
         <v>201</v>
       </c>
-      <c r="C70" s="30" t="s">
+      <c r="C70" s="124" t="s">
         <v>202</v>
       </c>
       <c r="D70" s="22" t="s">
@@ -15602,9 +15665,9 @@
       <c r="BI70" s="24"/>
     </row>
     <row r="71" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A71" s="70"/>
-      <c r="B71" s="72"/>
-      <c r="C71" s="30" t="s">
+      <c r="A71" s="98"/>
+      <c r="B71" s="135"/>
+      <c r="C71" s="124" t="s">
         <v>204</v>
       </c>
       <c r="D71" s="22" t="s">
@@ -15669,11 +15732,11 @@
       <c r="BI71" s="24"/>
     </row>
     <row r="72" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A72" s="70"/>
-      <c r="B72" s="40" t="s">
+      <c r="A72" s="98"/>
+      <c r="B72" s="133" t="s">
         <v>206</v>
       </c>
-      <c r="C72" s="30" t="s">
+      <c r="C72" s="124" t="s">
         <v>207</v>
       </c>
       <c r="D72" s="22" t="s">
@@ -15738,11 +15801,11 @@
       <c r="BI72" s="24"/>
     </row>
     <row r="73" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A73" s="70"/>
-      <c r="B73" s="40" t="s">
+      <c r="A73" s="98"/>
+      <c r="B73" s="133" t="s">
         <v>209</v>
       </c>
-      <c r="C73" s="30" t="s">
+      <c r="C73" s="124" t="s">
         <v>210</v>
       </c>
       <c r="D73" s="22" t="s">
@@ -15807,11 +15870,11 @@
       <c r="BI73" s="24"/>
     </row>
     <row r="74" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A74" s="70"/>
-      <c r="B74" s="40" t="s">
+      <c r="A74" s="98"/>
+      <c r="B74" s="133" t="s">
         <v>212</v>
       </c>
-      <c r="C74" s="30" t="s">
+      <c r="C74" s="124" t="s">
         <v>213</v>
       </c>
       <c r="D74" s="22" t="s">
@@ -15876,11 +15939,11 @@
       <c r="BI74" s="24"/>
     </row>
     <row r="75" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A75" s="70"/>
-      <c r="B75" s="72" t="s">
+      <c r="A75" s="98"/>
+      <c r="B75" s="135" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="44" t="s">
+      <c r="C75" s="136" t="s">
         <v>216</v>
       </c>
       <c r="D75" s="22" t="s">
@@ -15945,9 +16008,9 @@
       <c r="BI75" s="24"/>
     </row>
     <row r="76" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A76" s="70"/>
-      <c r="B76" s="72"/>
-      <c r="C76" s="44" t="s">
+      <c r="A76" s="98"/>
+      <c r="B76" s="135"/>
+      <c r="C76" s="136" t="s">
         <v>218</v>
       </c>
       <c r="D76" s="22" t="s">
@@ -16012,9 +16075,9 @@
       <c r="BI76" s="24"/>
     </row>
     <row r="77" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A77" s="70"/>
-      <c r="B77" s="72"/>
-      <c r="C77" s="44" t="s">
+      <c r="A77" s="98"/>
+      <c r="B77" s="135"/>
+      <c r="C77" s="136" t="s">
         <v>220</v>
       </c>
       <c r="D77" s="22" t="s">
@@ -16079,11 +16142,11 @@
       <c r="BI77" s="24"/>
     </row>
     <row r="78" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A78" s="71"/>
-      <c r="B78" s="45" t="s">
+      <c r="A78" s="97"/>
+      <c r="B78" s="137" t="s">
         <v>222</v>
       </c>
-      <c r="C78" s="44" t="s">
+      <c r="C78" s="136" t="s">
         <v>223</v>
       </c>
       <c r="D78" s="22" t="s">
@@ -16148,13 +16211,13 @@
       <c r="BI78" s="24"/>
     </row>
     <row r="79" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A79" s="69" t="s">
+      <c r="A79" s="96" t="s">
         <v>225</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B79" s="127" t="s">
         <v>226</v>
       </c>
-      <c r="C79" s="30" t="s">
+      <c r="C79" s="124" t="s">
         <v>227</v>
       </c>
       <c r="D79" s="22" t="s">
@@ -16219,9 +16282,9 @@
       <c r="BI79" s="24"/>
     </row>
     <row r="80" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A80" s="70"/>
-      <c r="B80" s="74"/>
-      <c r="C80" s="30" t="s">
+      <c r="A80" s="98"/>
+      <c r="B80" s="129"/>
+      <c r="C80" s="124" t="s">
         <v>229</v>
       </c>
       <c r="D80" s="22" t="s">
@@ -16286,11 +16349,11 @@
       <c r="BI80" s="24"/>
     </row>
     <row r="81" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A81" s="70"/>
-      <c r="B81" s="29" t="s">
+      <c r="A81" s="98"/>
+      <c r="B81" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="C81" s="30" t="s">
+      <c r="C81" s="124" t="s">
         <v>232</v>
       </c>
       <c r="D81" s="22" t="s">
@@ -16355,11 +16418,11 @@
       <c r="BI81" s="24"/>
     </row>
     <row r="82" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A82" s="70"/>
-      <c r="B82" s="72" t="s">
+      <c r="A82" s="98"/>
+      <c r="B82" s="135" t="s">
         <v>234</v>
       </c>
-      <c r="C82" s="44" t="s">
+      <c r="C82" s="136" t="s">
         <v>235</v>
       </c>
       <c r="D82" s="22" t="s">
@@ -16424,9 +16487,9 @@
       <c r="BI82" s="24"/>
     </row>
     <row r="83" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A83" s="70"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="44" t="s">
+      <c r="A83" s="98"/>
+      <c r="B83" s="135"/>
+      <c r="C83" s="136" t="s">
         <v>237</v>
       </c>
       <c r="D83" s="22" t="s">
@@ -16491,11 +16554,11 @@
       <c r="BI83" s="24"/>
     </row>
     <row r="84" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A84" s="70"/>
-      <c r="B84" s="45" t="s">
+      <c r="A84" s="98"/>
+      <c r="B84" s="137" t="s">
         <v>239</v>
       </c>
-      <c r="C84" s="44" t="s">
+      <c r="C84" s="136" t="s">
         <v>240</v>
       </c>
       <c r="D84" s="22" t="s">
@@ -16560,11 +16623,11 @@
       <c r="BI84" s="24"/>
     </row>
     <row r="85" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A85" s="70"/>
-      <c r="B85" s="73" t="s">
+      <c r="A85" s="98"/>
+      <c r="B85" s="127" t="s">
         <v>242</v>
       </c>
-      <c r="C85" s="44" t="s">
+      <c r="C85" s="136" t="s">
         <v>243</v>
       </c>
       <c r="D85" s="22" t="s">
@@ -16629,9 +16692,9 @@
       <c r="BI85" s="24"/>
     </row>
     <row r="86" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A86" s="70"/>
-      <c r="B86" s="75"/>
-      <c r="C86" s="44" t="s">
+      <c r="A86" s="98"/>
+      <c r="B86" s="128"/>
+      <c r="C86" s="136" t="s">
         <v>245</v>
       </c>
       <c r="D86" s="22" t="s">
@@ -16696,9 +16759,9 @@
       <c r="BI86" s="24"/>
     </row>
     <row r="87" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A87" s="70"/>
-      <c r="B87" s="74"/>
-      <c r="C87" s="44" t="s">
+      <c r="A87" s="98"/>
+      <c r="B87" s="129"/>
+      <c r="C87" s="136" t="s">
         <v>247</v>
       </c>
       <c r="D87" s="22" t="s">
@@ -16763,11 +16826,11 @@
       <c r="BI87" s="24"/>
     </row>
     <row r="88" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A88" s="70"/>
-      <c r="B88" s="45" t="s">
+      <c r="A88" s="98"/>
+      <c r="B88" s="137" t="s">
         <v>249</v>
       </c>
-      <c r="C88" s="44" t="s">
+      <c r="C88" s="136" t="s">
         <v>250</v>
       </c>
       <c r="D88" s="22" t="s">
@@ -16832,11 +16895,11 @@
       <c r="BI88" s="24"/>
     </row>
     <row r="89" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A89" s="70"/>
-      <c r="B89" s="73" t="s">
+      <c r="A89" s="98"/>
+      <c r="B89" s="127" t="s">
         <v>252</v>
       </c>
-      <c r="C89" s="44" t="s">
+      <c r="C89" s="136" t="s">
         <v>253</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -16901,9 +16964,9 @@
       <c r="BI89" s="24"/>
     </row>
     <row r="90" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A90" s="70"/>
-      <c r="B90" s="75"/>
-      <c r="C90" s="44" t="s">
+      <c r="A90" s="98"/>
+      <c r="B90" s="128"/>
+      <c r="C90" s="136" t="s">
         <v>255</v>
       </c>
       <c r="D90" s="22" t="s">
@@ -16968,9 +17031,9 @@
       <c r="BI90" s="24"/>
     </row>
     <row r="91" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A91" s="70"/>
-      <c r="B91" s="75"/>
-      <c r="C91" s="44" t="s">
+      <c r="A91" s="98"/>
+      <c r="B91" s="128"/>
+      <c r="C91" s="136" t="s">
         <v>245</v>
       </c>
       <c r="D91" s="22" t="s">
@@ -17035,9 +17098,9 @@
       <c r="BI91" s="24"/>
     </row>
     <row r="92" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A92" s="71"/>
-      <c r="B92" s="74"/>
-      <c r="C92" s="44" t="s">
+      <c r="A92" s="97"/>
+      <c r="B92" s="129"/>
+      <c r="C92" s="136" t="s">
         <v>247</v>
       </c>
       <c r="D92" s="22" t="s">
@@ -17102,13 +17165,13 @@
       <c r="BI92" s="24"/>
     </row>
     <row r="93" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A93" s="69" t="s">
+      <c r="A93" s="96" t="s">
         <v>257</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B93" s="127" t="s">
         <v>258</v>
       </c>
-      <c r="C93" s="44" t="s">
+      <c r="C93" s="136" t="s">
         <v>259</v>
       </c>
       <c r="D93" s="22" t="s">
@@ -17173,9 +17236,9 @@
       <c r="BI93" s="24"/>
     </row>
     <row r="94" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A94" s="71"/>
-      <c r="B94" s="74"/>
-      <c r="C94" s="44" t="s">
+      <c r="A94" s="97"/>
+      <c r="B94" s="129"/>
+      <c r="C94" s="136" t="s">
         <v>261</v>
       </c>
       <c r="D94" s="22" t="s">
@@ -17303,13 +17366,13 @@
       <c r="BI95" s="26"/>
     </row>
     <row r="96" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A96" s="69" t="s">
+      <c r="A96" s="96" t="s">
         <v>263</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="135" t="s">
         <v>264</v>
       </c>
-      <c r="C96" s="44" t="s">
+      <c r="C96" s="136" t="s">
         <v>265</v>
       </c>
       <c r="D96" s="22" t="s">
@@ -17374,9 +17437,9 @@
       <c r="BI96" s="24"/>
     </row>
     <row r="97" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A97" s="70"/>
-      <c r="B97" s="72"/>
-      <c r="C97" s="44" t="s">
+      <c r="A97" s="98"/>
+      <c r="B97" s="135"/>
+      <c r="C97" s="136" t="s">
         <v>267</v>
       </c>
       <c r="D97" s="22" t="s">
@@ -17441,11 +17504,11 @@
       <c r="BI97" s="24"/>
     </row>
     <row r="98" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="71"/>
-      <c r="B98" s="41" t="s">
+      <c r="A98" s="97"/>
+      <c r="B98" s="134" t="s">
         <v>269</v>
       </c>
-      <c r="C98" s="44" t="s">
+      <c r="C98" s="136" t="s">
         <v>270</v>
       </c>
       <c r="D98" s="22" t="s">
@@ -17509,13 +17572,13 @@
       <c r="BI98" s="24"/>
     </row>
     <row r="99" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A99" s="69" t="s">
+      <c r="A99" s="96" t="s">
         <v>272</v>
       </c>
-      <c r="B99" s="45" t="s">
+      <c r="B99" s="137" t="s">
         <v>273</v>
       </c>
-      <c r="C99" s="44" t="s">
+      <c r="C99" s="136" t="s">
         <v>274</v>
       </c>
       <c r="D99" s="22" t="s">
@@ -17580,11 +17643,11 @@
       <c r="BI99" s="24"/>
     </row>
     <row r="100" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A100" s="70"/>
-      <c r="B100" s="41" t="s">
+      <c r="A100" s="98"/>
+      <c r="B100" s="134" t="s">
         <v>276</v>
       </c>
-      <c r="C100" s="44" t="s">
+      <c r="C100" s="136" t="s">
         <v>277</v>
       </c>
       <c r="D100" s="22" t="s">
@@ -17649,11 +17712,11 @@
       <c r="BI100" s="24"/>
     </row>
     <row r="101" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="71"/>
-      <c r="B101" s="41" t="s">
+      <c r="A101" s="97"/>
+      <c r="B101" s="134" t="s">
         <v>279</v>
       </c>
-      <c r="C101" s="44" t="s">
+      <c r="C101" s="136" t="s">
         <v>280</v>
       </c>
       <c r="D101" s="46" t="s">
@@ -17718,13 +17781,13 @@
       <c r="BI101" s="24"/>
     </row>
     <row r="102" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="69" t="s">
+      <c r="A102" s="96" t="s">
         <v>282</v>
       </c>
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="C102" s="44" t="s">
+      <c r="C102" s="136" t="s">
         <v>284</v>
       </c>
       <c r="D102" s="46" t="s">
@@ -17789,11 +17852,11 @@
       <c r="BI102" s="24"/>
     </row>
     <row r="103" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A103" s="71"/>
-      <c r="B103" s="41" t="s">
+      <c r="A103" s="97"/>
+      <c r="B103" s="134" t="s">
         <v>286</v>
       </c>
-      <c r="C103" s="44" t="s">
+      <c r="C103" s="136" t="s">
         <v>287</v>
       </c>
       <c r="D103" s="22" t="s">
@@ -17921,13 +17984,13 @@
       <c r="BI104" s="26"/>
     </row>
     <row r="105" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A105" s="69" t="s">
+      <c r="A105" s="96" t="s">
         <v>289</v>
       </c>
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="133" t="s">
         <v>290</v>
       </c>
-      <c r="C105" s="30" t="s">
+      <c r="C105" s="124" t="s">
         <v>291</v>
       </c>
       <c r="D105" s="22" t="s">
@@ -17992,11 +18055,11 @@
       <c r="BI105" s="24"/>
     </row>
     <row r="106" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A106" s="70"/>
-      <c r="B106" s="40" t="s">
+      <c r="A106" s="98"/>
+      <c r="B106" s="133" t="s">
         <v>293</v>
       </c>
-      <c r="C106" s="30" t="s">
+      <c r="C106" s="124" t="s">
         <v>294</v>
       </c>
       <c r="D106" s="22" t="s">
@@ -18061,11 +18124,11 @@
       <c r="BI106" s="24"/>
     </row>
     <row r="107" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A107" s="70"/>
-      <c r="B107" s="40" t="s">
+      <c r="A107" s="98"/>
+      <c r="B107" s="133" t="s">
         <v>296</v>
       </c>
-      <c r="C107" s="30" t="s">
+      <c r="C107" s="124" t="s">
         <v>297</v>
       </c>
       <c r="D107" s="22" t="s">
@@ -18130,11 +18193,11 @@
       <c r="BI107" s="24"/>
     </row>
     <row r="108" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A108" s="70"/>
-      <c r="B108" s="72" t="s">
+      <c r="A108" s="98"/>
+      <c r="B108" s="135" t="s">
         <v>299</v>
       </c>
-      <c r="C108" s="44" t="s">
+      <c r="C108" s="136" t="s">
         <v>300</v>
       </c>
       <c r="D108" s="22" t="s">
@@ -18199,9 +18262,9 @@
       <c r="BI108" s="24"/>
     </row>
     <row r="109" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A109" s="70"/>
-      <c r="B109" s="72"/>
-      <c r="C109" s="44" t="s">
+      <c r="A109" s="98"/>
+      <c r="B109" s="135"/>
+      <c r="C109" s="136" t="s">
         <v>302</v>
       </c>
       <c r="D109" s="22" t="s">
@@ -18266,9 +18329,9 @@
       <c r="BI109" s="24"/>
     </row>
     <row r="110" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A110" s="70"/>
-      <c r="B110" s="72"/>
-      <c r="C110" s="44" t="s">
+      <c r="A110" s="98"/>
+      <c r="B110" s="135"/>
+      <c r="C110" s="136" t="s">
         <v>304</v>
       </c>
       <c r="D110" s="22" t="s">
@@ -18333,11 +18396,11 @@
       <c r="BI110" s="24"/>
     </row>
     <row r="111" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A111" s="70"/>
-      <c r="B111" s="72" t="s">
+      <c r="A111" s="98"/>
+      <c r="B111" s="135" t="s">
         <v>306</v>
       </c>
-      <c r="C111" s="44" t="s">
+      <c r="C111" s="136" t="s">
         <v>307</v>
       </c>
       <c r="D111" s="22" t="s">
@@ -18402,9 +18465,9 @@
       <c r="BI111" s="24"/>
     </row>
     <row r="112" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A112" s="70"/>
-      <c r="B112" s="72"/>
-      <c r="C112" s="44" t="s">
+      <c r="A112" s="98"/>
+      <c r="B112" s="135"/>
+      <c r="C112" s="136" t="s">
         <v>309</v>
       </c>
       <c r="D112" s="22" t="s">
@@ -18469,11 +18532,11 @@
       <c r="BI112" s="24"/>
     </row>
     <row r="113" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A113" s="70"/>
-      <c r="B113" s="40" t="s">
+      <c r="A113" s="98"/>
+      <c r="B113" s="133" t="s">
         <v>311</v>
       </c>
-      <c r="C113" s="44" t="s">
+      <c r="C113" s="136" t="s">
         <v>312</v>
       </c>
       <c r="D113" s="22" t="s">
@@ -18538,11 +18601,11 @@
       <c r="BI113" s="24"/>
     </row>
     <row r="114" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A114" s="70"/>
-      <c r="B114" s="73" t="s">
+      <c r="A114" s="98"/>
+      <c r="B114" s="127" t="s">
         <v>314</v>
       </c>
-      <c r="C114" s="44" t="s">
+      <c r="C114" s="136" t="s">
         <v>315</v>
       </c>
       <c r="D114" s="22" t="s">
@@ -18607,9 +18670,9 @@
       <c r="BI114" s="24"/>
     </row>
     <row r="115" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A115" s="70"/>
-      <c r="B115" s="74"/>
-      <c r="C115" s="44" t="s">
+      <c r="A115" s="98"/>
+      <c r="B115" s="129"/>
+      <c r="C115" s="136" t="s">
         <v>317</v>
       </c>
       <c r="D115" s="47" t="s">
@@ -18674,11 +18737,11 @@
       <c r="BI115" s="24"/>
     </row>
     <row r="116" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A116" s="71"/>
-      <c r="B116" s="40" t="s">
+      <c r="A116" s="97"/>
+      <c r="B116" s="133" t="s">
         <v>319</v>
       </c>
-      <c r="C116" s="44" t="s">
+      <c r="C116" s="136" t="s">
         <v>320</v>
       </c>
       <c r="D116" s="22" t="s">
@@ -18743,18 +18806,18 @@
       <c r="BI116" s="24"/>
     </row>
     <row r="118" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B118" s="65" t="s">
+      <c r="B118" s="102" t="s">
         <v>322</v>
       </c>
-      <c r="C118" s="65"/>
-      <c r="D118" s="65"/>
-      <c r="E118" s="65"/>
-      <c r="F118" s="65"/>
-      <c r="G118" s="65"/>
-      <c r="H118" s="65"/>
-      <c r="I118" s="65"/>
-      <c r="J118" s="65"/>
-      <c r="K118" s="65"/>
+      <c r="C118" s="102"/>
+      <c r="D118" s="102"/>
+      <c r="E118" s="102"/>
+      <c r="F118" s="102"/>
+      <c r="G118" s="102"/>
+      <c r="H118" s="102"/>
+      <c r="I118" s="102"/>
+      <c r="J118" s="102"/>
+      <c r="K118" s="102"/>
       <c r="L118" s="48"/>
       <c r="M118" s="48"/>
       <c r="N118" s="48"/>
@@ -18774,72 +18837,61 @@
       <c r="AB118" s="48"/>
     </row>
     <row r="119" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B119" s="66" t="s">
+      <c r="B119" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
+      <c r="C119" s="103"/>
+      <c r="D119" s="103"/>
+      <c r="E119" s="103"/>
+      <c r="F119" s="103"/>
+      <c r="G119" s="103"/>
+      <c r="H119" s="103"/>
+      <c r="I119" s="103"/>
+      <c r="J119" s="103"/>
+      <c r="K119" s="103"/>
     </row>
     <row r="120" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B120" s="67" t="s">
+      <c r="B120" s="104" t="s">
         <v>334</v>
       </c>
-      <c r="C120" s="67"/>
-      <c r="D120" s="67"/>
-      <c r="E120" s="67"/>
-      <c r="F120" s="67"/>
-      <c r="G120" s="67"/>
-      <c r="H120" s="67"/>
-      <c r="I120" s="67"/>
-      <c r="J120" s="67"/>
-      <c r="K120" s="67"/>
+      <c r="C120" s="104"/>
+      <c r="D120" s="104"/>
+      <c r="E120" s="104"/>
+      <c r="F120" s="104"/>
+      <c r="G120" s="104"/>
+      <c r="H120" s="104"/>
+      <c r="I120" s="104"/>
+      <c r="J120" s="104"/>
+      <c r="K120" s="104"/>
     </row>
     <row r="121" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B121" s="106" t="s">
+      <c r="B121" s="107" t="s">
         <v>325</v>
       </c>
-      <c r="C121" s="68"/>
-      <c r="D121" s="68"/>
-      <c r="E121" s="68"/>
-      <c r="F121" s="68"/>
-      <c r="G121" s="68"/>
-      <c r="H121" s="68"/>
-      <c r="I121" s="68"/>
-      <c r="J121" s="68"/>
-      <c r="K121" s="68"/>
+      <c r="C121" s="105"/>
+      <c r="D121" s="105"/>
+      <c r="E121" s="105"/>
+      <c r="F121" s="105"/>
+      <c r="G121" s="105"/>
+      <c r="H121" s="105"/>
+      <c r="I121" s="105"/>
+      <c r="J121" s="105"/>
+      <c r="K121" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="W1:AC1"/>
-    <mergeCell ref="AE1:AO1"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="A20:A50"/>
-    <mergeCell ref="B20:B39"/>
-    <mergeCell ref="B41:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B118:K118"/>
+    <mergeCell ref="B119:K119"/>
+    <mergeCell ref="B120:K120"/>
+    <mergeCell ref="B121:K121"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A105:A116"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B114:B115"/>
     <mergeCell ref="A93:A94"/>
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="A52:A57"/>
@@ -18856,18 +18908,29 @@
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B118:K118"/>
-    <mergeCell ref="B119:K119"/>
-    <mergeCell ref="B120:K120"/>
-    <mergeCell ref="B121:K121"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A105:A116"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A20:A50"/>
+    <mergeCell ref="B20:B39"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="AV1:AX1"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="AE1:AO1"/>
+    <mergeCell ref="AQ1:AT1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18909,119 +18972,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A1" s="107"/>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
+      <c r="A1" s="106"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
       <c r="D1" s="64" t="s">
         <v>326</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="87" t="s">
+      <c r="W1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="100" t="s">
+      <c r="AE1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="101"/>
-      <c r="AH1" s="101"/>
-      <c r="AI1" s="101"/>
-      <c r="AJ1" s="101"/>
-      <c r="AK1" s="101"/>
-      <c r="AL1" s="101"/>
-      <c r="AM1" s="101"/>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="102"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="78"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="103" t="s">
+      <c r="AQ1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="AR1" s="104"/>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="105"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="81"/>
       <c r="AU1" s="1"/>
-      <c r="AV1" s="87" t="s">
+      <c r="AV1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
       <c r="AY1" s="1"/>
-      <c r="AZ1" s="88" t="s">
+      <c r="AZ1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="89"/>
-      <c r="BC1" s="89"/>
+      <c r="BA1" s="66"/>
+      <c r="BB1" s="66"/>
+      <c r="BC1" s="66"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="BF1" s="1"/>
-      <c r="BG1" s="87" t="s">
+      <c r="BG1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="BH1" s="87"/>
-      <c r="BI1" s="87"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="68"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="64" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="107">
+      <c r="E2" s="106">
         <v>1</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="106"/>
       <c r="G2" s="49">
         <v>2</v>
       </c>
       <c r="H2" s="49">
         <v>3</v>
       </c>
-      <c r="I2" s="107">
+      <c r="I2" s="106">
         <v>4</v>
       </c>
-      <c r="J2" s="107"/>
+      <c r="J2" s="106"/>
       <c r="K2" s="49">
         <v>5</v>
       </c>
       <c r="L2" s="49">
         <v>6</v>
       </c>
-      <c r="M2" s="107">
+      <c r="M2" s="106">
         <v>7</v>
       </c>
-      <c r="N2" s="107"/>
+      <c r="N2" s="106"/>
       <c r="O2" s="49">
         <v>8</v>
       </c>
@@ -19032,10 +19095,10 @@
         <v>10</v>
       </c>
       <c r="R2" s="5"/>
-      <c r="S2" s="107">
+      <c r="S2" s="106">
         <v>1</v>
       </c>
-      <c r="T2" s="107"/>
+      <c r="T2" s="106"/>
       <c r="U2" s="49">
         <v>2</v>
       </c>
@@ -19049,11 +19112,11 @@
       <c r="Y2" s="49">
         <v>3</v>
       </c>
-      <c r="Z2" s="107">
+      <c r="Z2" s="106">
         <v>4</v>
       </c>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
       <c r="AC2" s="49">
         <v>5</v>
       </c>
@@ -19143,9 +19206,9 @@
       </c>
     </row>
     <row r="3" spans="1:61" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="107"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
+      <c r="A3" s="106"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
       <c r="D3" s="64" t="s">
         <v>331</v>
       </c>
@@ -19447,11 +19510,11 @@
         <v>50</v>
       </c>
       <c r="AY4" s="18"/>
-      <c r="AZ4" s="79" t="s">
+      <c r="AZ4" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="80"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="95"/>
       <c r="BC4" s="50" t="s">
         <v>52</v>
       </c>
@@ -19471,10 +19534,10 @@
       </c>
     </row>
     <row r="5" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="114">
+      <c r="B5" s="109">
         <v>1</v>
       </c>
       <c r="C5" s="24">
@@ -19542,8 +19605,8 @@
       <c r="BI5" s="25"/>
     </row>
     <row r="6" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="111"/>
-      <c r="B6" s="114"/>
+      <c r="A6" s="108"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="24">
         <v>2</v>
       </c>
@@ -19609,7 +19672,7 @@
       <c r="BI6" s="25"/>
     </row>
     <row r="7" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="111"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="24">
         <v>2</v>
       </c>
@@ -19678,7 +19741,7 @@
       <c r="BI7" s="25"/>
     </row>
     <row r="8" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="111"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="24">
         <v>3</v>
       </c>
@@ -19747,8 +19810,8 @@
       <c r="BI8" s="25"/>
     </row>
     <row r="9" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="111"/>
-      <c r="B9" s="114">
+      <c r="A9" s="108"/>
+      <c r="B9" s="109">
         <v>4</v>
       </c>
       <c r="C9" s="24">
@@ -19816,8 +19879,8 @@
       <c r="BI9" s="25"/>
     </row>
     <row r="10" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="111"/>
-      <c r="B10" s="114"/>
+      <c r="A10" s="108"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="24">
         <v>2</v>
       </c>
@@ -19883,7 +19946,7 @@
       <c r="BI10" s="24"/>
     </row>
     <row r="11" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="111"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="24">
         <v>5</v>
       </c>
@@ -19952,7 +20015,7 @@
       <c r="BI11" s="24"/>
     </row>
     <row r="12" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="111"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="24">
         <v>6</v>
       </c>
@@ -20021,8 +20084,8 @@
       <c r="BI12" s="24"/>
     </row>
     <row r="13" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="111"/>
-      <c r="B13" s="114">
+      <c r="A13" s="108"/>
+      <c r="B13" s="109">
         <v>7</v>
       </c>
       <c r="C13" s="24">
@@ -20090,8 +20153,8 @@
       <c r="BI13" s="25"/>
     </row>
     <row r="14" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="111"/>
-      <c r="B14" s="114"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="24">
         <v>2</v>
       </c>
@@ -20157,7 +20220,7 @@
       <c r="BI14" s="24"/>
     </row>
     <row r="15" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="111"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="24">
         <v>8</v>
       </c>
@@ -20226,7 +20289,7 @@
       <c r="BI15" s="24"/>
     </row>
     <row r="16" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="111"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="24">
         <v>9</v>
       </c>
@@ -20295,7 +20358,7 @@
       <c r="BI16" s="24"/>
     </row>
     <row r="17" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="111"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="24">
         <v>10</v>
       </c>
@@ -20427,10 +20490,10 @@
       <c r="BI18" s="58"/>
     </row>
     <row r="19" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="114">
+      <c r="B19" s="109">
         <v>1</v>
       </c>
       <c r="C19" s="24">
@@ -20498,8 +20561,8 @@
       <c r="BI19" s="24"/>
     </row>
     <row r="20" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="111"/>
-      <c r="B20" s="114"/>
+      <c r="A20" s="108"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="24">
         <v>2</v>
       </c>
@@ -20565,7 +20628,7 @@
       <c r="BI20" s="24"/>
     </row>
     <row r="21" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="111"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="24">
         <v>2</v>
       </c>
@@ -20697,7 +20760,7 @@
       <c r="BI22" s="58"/>
     </row>
     <row r="23" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="111" t="s">
+      <c r="A23" s="108" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="24">
@@ -20768,7 +20831,7 @@
       <c r="BI23" s="24"/>
     </row>
     <row r="24" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="111"/>
+      <c r="A24" s="108"/>
       <c r="B24" s="24">
         <v>2</v>
       </c>
@@ -20837,7 +20900,7 @@
       <c r="BI24" s="24"/>
     </row>
     <row r="25" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="111"/>
+      <c r="A25" s="108"/>
       <c r="B25" s="24">
         <v>3</v>
       </c>
@@ -20906,8 +20969,8 @@
       <c r="BI25" s="24"/>
     </row>
     <row r="26" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="111"/>
-      <c r="B26" s="114">
+      <c r="A26" s="108"/>
+      <c r="B26" s="109">
         <v>4</v>
       </c>
       <c r="C26" s="24">
@@ -20975,8 +21038,8 @@
       <c r="BI26" s="24"/>
     </row>
     <row r="27" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="111"/>
-      <c r="B27" s="114"/>
+      <c r="A27" s="108"/>
+      <c r="B27" s="109"/>
       <c r="C27" s="24">
         <v>2</v>
       </c>
@@ -21042,8 +21105,8 @@
       <c r="BI27" s="24"/>
     </row>
     <row r="28" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="111"/>
-      <c r="B28" s="114"/>
+      <c r="A28" s="108"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="24">
         <v>3</v>
       </c>
@@ -21109,7 +21172,7 @@
       <c r="BI28" s="24"/>
     </row>
     <row r="29" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="111"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="24">
         <v>5</v>
       </c>
@@ -21241,7 +21304,7 @@
       <c r="BI30" s="58"/>
     </row>
     <row r="31" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="115" t="s">
+      <c r="A31" s="110" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="24">
@@ -21312,7 +21375,7 @@
       <c r="BI31" s="24"/>
     </row>
     <row r="32" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="116"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="24">
         <v>2</v>
       </c>
@@ -21381,7 +21444,7 @@
       <c r="BI32" s="24"/>
     </row>
     <row r="33" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="116"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="24">
         <v>3</v>
       </c>
@@ -21450,7 +21513,7 @@
       <c r="BI33" s="24"/>
     </row>
     <row r="34" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="116"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="24">
         <v>4</v>
       </c>
@@ -21519,7 +21582,7 @@
       <c r="BI34" s="24"/>
     </row>
     <row r="35" spans="1:61" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="116"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="24">
         <v>5</v>
       </c>
@@ -21588,7 +21651,7 @@
       <c r="BI35" s="24"/>
     </row>
     <row r="36" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="116"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="24">
         <v>6</v>
       </c>
@@ -21657,7 +21720,7 @@
       <c r="BI36" s="24"/>
     </row>
     <row r="37" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="116"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="24">
         <v>7</v>
       </c>
@@ -21726,7 +21789,7 @@
       <c r="BI37" s="24"/>
     </row>
     <row r="38" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="116"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="24">
         <v>8</v>
       </c>
@@ -21795,7 +21858,7 @@
       <c r="BI38" s="24"/>
     </row>
     <row r="39" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="116"/>
+      <c r="A39" s="111"/>
       <c r="B39" s="24">
         <v>9</v>
       </c>
@@ -21864,7 +21927,7 @@
       <c r="BI39" s="24"/>
     </row>
     <row r="40" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="116"/>
+      <c r="A40" s="111"/>
       <c r="B40" s="24">
         <v>10</v>
       </c>
@@ -21933,7 +21996,7 @@
       <c r="BI40" s="24"/>
     </row>
     <row r="41" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="117"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="24">
         <v>11</v>
       </c>
@@ -22065,7 +22128,7 @@
       <c r="BI42" s="58"/>
     </row>
     <row r="43" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="24">
@@ -22136,7 +22199,7 @@
       <c r="BI43" s="24"/>
     </row>
     <row r="44" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="82"/>
+      <c r="A44" s="83"/>
       <c r="B44" s="24">
         <v>2</v>
       </c>
@@ -22205,7 +22268,7 @@
       <c r="BI44" s="24"/>
     </row>
     <row r="45" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="82"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="24">
         <v>3</v>
       </c>
@@ -22274,7 +22337,7 @@
       <c r="BI45" s="24"/>
     </row>
     <row r="46" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="83"/>
+      <c r="A46" s="84"/>
       <c r="B46" s="24">
         <v>4</v>
       </c>
@@ -22406,7 +22469,7 @@
       <c r="BI47" s="58"/>
     </row>
     <row r="48" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="111" t="s">
+      <c r="A48" s="108" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="24">
@@ -22477,7 +22540,7 @@
       <c r="BI48" s="24"/>
     </row>
     <row r="49" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="111"/>
+      <c r="A49" s="108"/>
       <c r="B49" s="24">
         <v>2</v>
       </c>
@@ -22546,7 +22609,7 @@
       <c r="BI49" s="24"/>
     </row>
     <row r="50" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="111"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="24">
         <v>3</v>
       </c>
@@ -22678,7 +22741,7 @@
       <c r="BI51" s="26"/>
     </row>
     <row r="52" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="82" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="24">
@@ -22687,7 +22750,7 @@
       <c r="C52" s="24">
         <v>1</v>
       </c>
-      <c r="D52" s="108" t="s">
+      <c r="D52" s="113" t="s">
         <v>51</v>
       </c>
       <c r="E52" s="23"/>
@@ -22749,14 +22812,14 @@
       <c r="BI52" s="24"/>
     </row>
     <row r="53" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="82"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="24">
         <v>2</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="109"/>
+      <c r="D53" s="114"/>
       <c r="E53" s="23"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
@@ -22816,14 +22879,14 @@
       <c r="BI53" s="24"/>
     </row>
     <row r="54" spans="1:61" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="82"/>
+      <c r="A54" s="83"/>
       <c r="B54" s="24">
         <v>3</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="110"/>
+      <c r="D54" s="115"/>
       <c r="E54" s="23"/>
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
@@ -22883,7 +22946,7 @@
       <c r="BI54" s="24"/>
     </row>
     <row r="55" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="83"/>
+      <c r="A55" s="84"/>
       <c r="B55" s="24">
         <v>4</v>
       </c>
@@ -23149,7 +23212,7 @@
       <c r="BI58" s="26"/>
     </row>
     <row r="59" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="111" t="s">
+      <c r="A59" s="108" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="24">
@@ -23220,7 +23283,7 @@
       <c r="BI59" s="24"/>
     </row>
     <row r="60" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="111"/>
+      <c r="A60" s="108"/>
       <c r="B60" s="24">
         <v>2</v>
       </c>
@@ -23289,7 +23352,7 @@
       <c r="BI60" s="24"/>
     </row>
     <row r="61" spans="1:61" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="111"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="24">
         <v>3</v>
       </c>
@@ -23358,60 +23421,60 @@
       <c r="BI61" s="24"/>
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="D63" s="112" t="s">
+      <c r="D63" s="116" t="s">
         <v>322</v>
       </c>
-      <c r="E63" s="112"/>
-      <c r="F63" s="112"/>
-      <c r="G63" s="112"/>
-      <c r="H63" s="112"/>
-      <c r="I63" s="112"/>
-      <c r="J63" s="112"/>
-      <c r="K63" s="112"/>
-      <c r="L63" s="112"/>
-      <c r="M63" s="112"/>
+      <c r="E63" s="116"/>
+      <c r="F63" s="116"/>
+      <c r="G63" s="116"/>
+      <c r="H63" s="116"/>
+      <c r="I63" s="116"/>
+      <c r="J63" s="116"/>
+      <c r="K63" s="116"/>
+      <c r="L63" s="116"/>
+      <c r="M63" s="116"/>
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="D64" s="66" t="s">
+      <c r="D64" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="66"/>
-      <c r="H64" s="66"/>
-      <c r="I64" s="66"/>
-      <c r="J64" s="66"/>
-      <c r="K64" s="66"/>
-      <c r="L64" s="66"/>
-      <c r="M64" s="66"/>
+      <c r="E64" s="103"/>
+      <c r="F64" s="103"/>
+      <c r="G64" s="103"/>
+      <c r="H64" s="103"/>
+      <c r="I64" s="103"/>
+      <c r="J64" s="103"/>
+      <c r="K64" s="103"/>
+      <c r="L64" s="103"/>
+      <c r="M64" s="103"/>
     </row>
     <row r="65" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D65" s="113" t="s">
+      <c r="D65" s="117" t="s">
         <v>332</v>
       </c>
-      <c r="E65" s="113"/>
-      <c r="F65" s="113"/>
-      <c r="G65" s="113"/>
-      <c r="H65" s="113"/>
-      <c r="I65" s="113"/>
-      <c r="J65" s="113"/>
-      <c r="K65" s="113"/>
-      <c r="L65" s="113"/>
-      <c r="M65" s="113"/>
+      <c r="E65" s="117"/>
+      <c r="F65" s="117"/>
+      <c r="G65" s="117"/>
+      <c r="H65" s="117"/>
+      <c r="I65" s="117"/>
+      <c r="J65" s="117"/>
+      <c r="K65" s="117"/>
+      <c r="L65" s="117"/>
+      <c r="M65" s="117"/>
     </row>
     <row r="66" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D66" s="68" t="s">
+      <c r="D66" s="105" t="s">
         <v>333</v>
       </c>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
-      <c r="I66" s="68"/>
-      <c r="J66" s="68"/>
-      <c r="K66" s="68"/>
-      <c r="L66" s="68"/>
-      <c r="M66" s="68"/>
+      <c r="E66" s="105"/>
+      <c r="F66" s="105"/>
+      <c r="G66" s="105"/>
+      <c r="H66" s="105"/>
+      <c r="I66" s="105"/>
+      <c r="J66" s="105"/>
+      <c r="K66" s="105"/>
+      <c r="L66" s="105"/>
+      <c r="M66" s="105"/>
     </row>
     <row r="68" spans="4:28" x14ac:dyDescent="0.2">
       <c r="E68" s="63"/>
@@ -23468,23 +23531,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A5:A17"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A31:A41"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="D66:M66"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="AZ4:BB4"/>
@@ -23501,6 +23547,23 @@
     <mergeCell ref="D64:M64"/>
     <mergeCell ref="D65:M65"/>
     <mergeCell ref="A23:A29"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A31:A41"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A5:A17"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>